<commit_message>
Entrega tarea 5 métodos computacionales
</commit_message>
<xml_diff>
--- a/otrasMaterias/Book1.xlsx
+++ b/otrasMaterias/Book1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javier\Desktop\2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javier\Desktop\2017\otrasMaterias\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8115"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Prácticas</t>
   </si>
@@ -42,6 +42,21 @@
   </si>
   <si>
     <t>Proyecto</t>
+  </si>
+  <si>
+    <t>Parciales</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Tarea</t>
+  </si>
+  <si>
+    <t>Definitivas</t>
+  </si>
+  <si>
+    <t>Computacionales</t>
   </si>
 </sst>
 </file>
@@ -393,15 +408,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H4:Q10"/>
+  <dimension ref="A4:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
         <v>0</v>
       </c>
@@ -424,7 +442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H5">
         <v>0.4</v>
       </c>
@@ -451,7 +469,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="6" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H6">
         <v>3.29</v>
       </c>
@@ -475,7 +493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H7">
         <f>H6*H5</f>
         <v>1.3160000000000001</v>
@@ -512,20 +530,181 @@
         <v>41.000000000000007</v>
       </c>
     </row>
-    <row r="8" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>4.3</v>
+      </c>
       <c r="O8">
         <v>4.5</v>
       </c>
     </row>
-    <row r="9" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4.7</v>
+      </c>
       <c r="O9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>4.2</v>
+      </c>
       <c r="O10">
         <f>AVERAGE(O5:O9)</f>
         <v>2.7800000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3.4</v>
+      </c>
+      <c r="O12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>AVERAGE(E18:G18)</f>
+        <v>3.8666666666666667</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4.07</v>
+      </c>
+      <c r="B14">
+        <v>75</v>
+      </c>
+      <c r="C14">
+        <f>AVERAGE(C8:C13)</f>
+        <v>3.9611111111111108</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+      <c r="H14">
+        <v>0.6</v>
+      </c>
+      <c r="I14">
+        <v>0.25</v>
+      </c>
+      <c r="J14">
+        <v>0.15</v>
+      </c>
+      <c r="K14">
+        <f>SUM(H14:J14)</f>
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>85</v>
+      </c>
+      <c r="P14">
+        <f>18/25</f>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>A14*B14</f>
+        <v>305.25</v>
+      </c>
+      <c r="B15">
+        <f>D14*C14</f>
+        <v>71.3</v>
+      </c>
+      <c r="C15">
+        <f>(B15+A15)/(D14+B14)</f>
+        <v>4.0489247311827956</v>
+      </c>
+      <c r="H15">
+        <v>4.2</v>
+      </c>
+      <c r="I15">
+        <f>24/29*5</f>
+        <v>4.1379310344827589</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="O15">
+        <v>100</v>
+      </c>
+      <c r="P15">
+        <f>P14*5</f>
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f>H15*H14</f>
+        <v>2.52</v>
+      </c>
+      <c r="I16">
+        <f>I15*I14</f>
+        <v>1.0344827586206897</v>
+      </c>
+      <c r="J16">
+        <f>J15*J14</f>
+        <v>0.75</v>
+      </c>
+      <c r="K16">
+        <f>SUM(H16:J16)</f>
+        <v>4.30448275862069</v>
+      </c>
+      <c r="O16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F18">
+        <v>3.4</v>
+      </c>
+      <c r="G18">
+        <v>3.6</v>
+      </c>
+      <c r="O18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <f>AVERAGE(O13:O18)*5/100</f>
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <f>O19+0.1*N19</f>
+        <v>4.7799999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>